<commit_message>
add test for guest crew, refactoring
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/templates/excel/event-details.xlsx
+++ b/backend/src/main/resources/templates/excel/event-details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte.schwitters/Projects/privat/eventplanner/backend/src/test/resources/templates/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte.schwitters/Projects/privat/eventplanner/backend/src/main/resources/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C4A8B7-E4E1-894E-93F3-A0FF4587B8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E459322-4A06-9D43-90E0-9AC1937408A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" activeTab="3" xr2:uid="{528125D0-B1E0-47D6-B7C9-C5F127A8A5B7}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{528125D0-B1E0-47D6-B7C9-C5F127A8A5B7}"/>
   </bookViews>
   <sheets>
     <sheet name="IMO Crewliste" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">Notfallinformationen!$A:$K</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Crew Qualifikationen'!$1:$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'IMO Crewliste'!$1:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Kombüseliste!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Kombüseliste!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">Notfallinformationen!$1:$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="84">
   <si>
     <t>Crew Informationen für den Kapitän</t>
   </si>
@@ -180,15 +180,6 @@
     <t>${renderQualificationExpiration(user, 'medical-care')}</t>
   </si>
   <si>
-    <t>${(user.diseases)!}</t>
-  </si>
-  <si>
-    <t>${(user.medication)!}</t>
-  </si>
-  <si>
-    <t>${(user.intolerances)!}</t>
-  </si>
-  <si>
     <t>${(user.emergencyContact.name)!}</t>
   </si>
   <si>
@@ -227,9 +218,6 @@
   </si>
   <si>
     <t>${renderQualificationList(user, fachqualifikationen)}</t>
-  </si>
-  <si>
-    <t>${(user.mobile)!}</t>
   </si>
   <si>
     <t>IMO CREW LIST</t>
@@ -289,15 +277,6 @@
     <t>11. Nature and No. of identity document</t>
   </si>
   <si>
-    <t>${(user.nationality)!}</t>
-  </si>
-  <si>
-    <t>${(user.placeOfBirth)!}</t>
-  </si>
-  <si>
-    <t>${(user.passNr)!}</t>
-  </si>
-  <si>
     <t>&lt;#assign i=row-8&gt;&lt;#assign user=(crew[i]!{}).user!{}&gt;&lt;#assign position=(crew[i]!{}).position!{}&gt;</t>
   </si>
   <si>
@@ -307,22 +286,67 @@
     <t>Crew Informationen für die Kombüse</t>
   </si>
   <si>
+    <t>${renderDiet(user)!}</t>
+  </si>
+  <si>
+    <t>${user.lastName!}</t>
+  </si>
+  <si>
+    <t>${user.intolerances!}</t>
+  </si>
+  <si>
+    <t>${user.intolerances!'}</t>
+  </si>
+  <si>
     <t>&lt;#function renderDiet user={}&gt;
-    &lt;#if user.firstName!?length == 0&gt;
+    &lt;#if user.lastName!?length == 0&gt;
         &lt;#return ''&gt;
-    &lt;#elseif user.diet == 'omnivore'&gt;
+    &lt;#elseif user.diet! == 'omnivore'&gt;
         &lt;#return 'Fleisch'&gt;
-    &lt;#elseif user.diet == 'vegan'&gt;
+    &lt;#elseif user.diet! == 'vegan'&gt;
         &lt;#return 'Vegan'&gt;
-    &lt;#elseif user.diet == 'vegetarian'&gt;
+    &lt;#elseif user.diet! == 'vegetarian'&gt;
         &lt;#return 'Vegetarisch'&gt;
     &lt;#else&gt;
-        &lt;#return user.diet!&gt;
+        &lt;#return ''&gt;
     &lt;/#if&gt;
 &lt;/#function&gt;</t>
   </si>
   <si>
-    <t>${renderDiet(user)!}</t>
+    <t>${user.firstNames!}</t>
+  </si>
+  <si>
+    <t>${position.imoListRank!}</t>
+  </si>
+  <si>
+    <t>${user.nationality!}</t>
+  </si>
+  <si>
+    <t>$(user.placeOfBirth!}</t>
+  </si>
+  <si>
+    <t>${user.passNr!}</t>
+  </si>
+  <si>
+    <t>${user.mobile!}</t>
+  </si>
+  <si>
+    <t>${user.diseases!}</t>
+  </si>
+  <si>
+    <t>${user.medication!}</t>
+  </si>
+  <si>
+    <t>Fleisch:</t>
+  </si>
+  <si>
+    <t>Vetegarisch</t>
+  </si>
+  <si>
+    <t>Vegan:</t>
+  </si>
+  <si>
+    <t>${user.nickName!user.firstName!} ${user.lastName!}</t>
   </si>
 </sst>
 </file>
@@ -907,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1090,14 +1114,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1118,6 +1139,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1246,11 +1276,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1690,7 +1730,7 @@
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1709,22 +1749,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
+      <c r="A1" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1735,7 +1775,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="37" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1747,13 +1787,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G3" s="35" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="31">
@@ -1761,121 +1801,121 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67" t="s">
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="36" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="72" t="s">
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="77"/>
+    </row>
+    <row r="7" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="52" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="75"/>
-    </row>
-    <row r="7" spans="1:10" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="75"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="77"/>
     </row>
     <row r="8" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="H8" s="59"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="60"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="38" x14ac:dyDescent="0.25">
       <c r="A9" s="45">
         <v>1</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="62"/>
+        <v>73</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="61"/>
       <c r="I9" s="47" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1892,14 +1932,14 @@
       <c r="D10" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="55"/>
+      <c r="E10" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="63"/>
+      <c r="G10" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="64"/>
       <c r="I10" s="50" t="s">
         <v>13</v>
       </c>
@@ -1921,14 +1961,14 @@
       <c r="D11" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="55"/>
+      <c r="E11" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="63"/>
+      <c r="G11" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="64"/>
       <c r="I11" s="50" t="s">
         <v>13</v>
       </c>
@@ -1950,14 +1990,14 @@
       <c r="D12" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="54"/>
-      <c r="G12" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="55"/>
+      <c r="E12" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="63"/>
+      <c r="G12" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="64"/>
       <c r="I12" s="50" t="s">
         <v>13</v>
       </c>
@@ -1979,14 +2019,14 @@
       <c r="D13" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="55"/>
+      <c r="E13" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="64"/>
       <c r="I13" s="50" t="s">
         <v>13</v>
       </c>
@@ -2008,14 +2048,14 @@
       <c r="D14" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="55"/>
+      <c r="E14" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="63"/>
+      <c r="G14" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="64"/>
       <c r="I14" s="50" t="s">
         <v>13</v>
       </c>
@@ -2037,14 +2077,14 @@
       <c r="D15" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="54"/>
-      <c r="G15" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="55"/>
+      <c r="E15" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="63"/>
+      <c r="G15" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="64"/>
       <c r="I15" s="50" t="s">
         <v>13</v>
       </c>
@@ -2066,14 +2106,14 @@
       <c r="D16" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="55"/>
+      <c r="E16" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="G16" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="64"/>
       <c r="I16" s="50" t="s">
         <v>13</v>
       </c>
@@ -2095,14 +2135,14 @@
       <c r="D17" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="55"/>
+      <c r="E17" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="63"/>
+      <c r="G17" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="64"/>
       <c r="I17" s="50" t="s">
         <v>13</v>
       </c>
@@ -2124,14 +2164,14 @@
       <c r="D18" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="55"/>
+      <c r="E18" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="64"/>
       <c r="I18" s="50" t="s">
         <v>13</v>
       </c>
@@ -2153,14 +2193,14 @@
       <c r="D19" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="55"/>
+      <c r="E19" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="63"/>
+      <c r="G19" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="64"/>
       <c r="I19" s="50" t="s">
         <v>13</v>
       </c>
@@ -2182,14 +2222,14 @@
       <c r="D20" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="55"/>
+      <c r="E20" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="63"/>
+      <c r="G20" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="64"/>
       <c r="I20" s="50" t="s">
         <v>13</v>
       </c>
@@ -2211,14 +2251,14 @@
       <c r="D21" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="54"/>
-      <c r="G21" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="55"/>
+      <c r="E21" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="64"/>
       <c r="I21" s="50" t="s">
         <v>13</v>
       </c>
@@ -2240,14 +2280,14 @@
       <c r="D22" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="55"/>
+      <c r="E22" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="63"/>
+      <c r="G22" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="64"/>
       <c r="I22" s="50" t="s">
         <v>13</v>
       </c>
@@ -2269,14 +2309,14 @@
       <c r="D23" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="54"/>
-      <c r="G23" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="55"/>
+      <c r="E23" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="63"/>
+      <c r="G23" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="64"/>
       <c r="I23" s="50" t="s">
         <v>13</v>
       </c>
@@ -2298,14 +2338,14 @@
       <c r="D24" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="54"/>
-      <c r="G24" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="55"/>
+      <c r="E24" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="63"/>
+      <c r="G24" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="64"/>
       <c r="I24" s="50" t="s">
         <v>13</v>
       </c>
@@ -2327,14 +2367,14 @@
       <c r="D25" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="54"/>
-      <c r="G25" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="55"/>
+      <c r="E25" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="63"/>
+      <c r="G25" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="64"/>
       <c r="I25" s="50" t="s">
         <v>13</v>
       </c>
@@ -2356,14 +2396,14 @@
       <c r="D26" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="54"/>
-      <c r="G26" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="55"/>
+      <c r="E26" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="64"/>
       <c r="I26" s="50" t="s">
         <v>13</v>
       </c>
@@ -2385,14 +2425,14 @@
       <c r="D27" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="54"/>
-      <c r="G27" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="55"/>
+      <c r="E27" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="64"/>
       <c r="I27" s="50" t="s">
         <v>13</v>
       </c>
@@ -2414,14 +2454,14 @@
       <c r="D28" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="54"/>
-      <c r="G28" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="55"/>
+      <c r="E28" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="64"/>
       <c r="I28" s="50" t="s">
         <v>13</v>
       </c>
@@ -2443,14 +2483,14 @@
       <c r="D29" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="54"/>
-      <c r="G29" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="55"/>
+      <c r="E29" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="63"/>
+      <c r="G29" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="64"/>
       <c r="I29" s="50" t="s">
         <v>13</v>
       </c>
@@ -2472,14 +2512,14 @@
       <c r="D30" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="54"/>
-      <c r="G30" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="55"/>
+      <c r="E30" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="63"/>
+      <c r="G30" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="64"/>
       <c r="I30" s="50" t="s">
         <v>13</v>
       </c>
@@ -2501,14 +2541,14 @@
       <c r="D31" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="54"/>
-      <c r="G31" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="55"/>
+      <c r="E31" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="63"/>
+      <c r="G31" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="64"/>
       <c r="I31" s="50" t="s">
         <v>13</v>
       </c>
@@ -2530,14 +2570,14 @@
       <c r="D32" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="54"/>
-      <c r="G32" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="55"/>
+      <c r="E32" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="63"/>
+      <c r="G32" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="64"/>
       <c r="I32" s="50" t="s">
         <v>13</v>
       </c>
@@ -2559,14 +2599,14 @@
       <c r="D33" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="54"/>
-      <c r="G33" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="55"/>
+      <c r="E33" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="63"/>
+      <c r="G33" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="64"/>
       <c r="I33" s="50" t="s">
         <v>13</v>
       </c>
@@ -2588,14 +2628,14 @@
       <c r="D34" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="54"/>
-      <c r="G34" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="55"/>
+      <c r="E34" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="63"/>
+      <c r="G34" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="64"/>
       <c r="I34" s="50" t="s">
         <v>13</v>
       </c>
@@ -2617,14 +2657,14 @@
       <c r="D35" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="54"/>
-      <c r="G35" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="55"/>
+      <c r="E35" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="63"/>
+      <c r="G35" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="64"/>
       <c r="I35" s="50" t="s">
         <v>13</v>
       </c>
@@ -2646,14 +2686,14 @@
       <c r="D36" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="54"/>
-      <c r="G36" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="55"/>
+      <c r="E36" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="63"/>
+      <c r="G36" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="64"/>
       <c r="I36" s="50" t="s">
         <v>13</v>
       </c>
@@ -2675,14 +2715,14 @@
       <c r="D37" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="54"/>
-      <c r="G37" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="55"/>
+      <c r="E37" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="63"/>
+      <c r="G37" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="64"/>
       <c r="I37" s="50" t="s">
         <v>13</v>
       </c>
@@ -2704,14 +2744,14 @@
       <c r="D38" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="54"/>
-      <c r="G38" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="55"/>
+      <c r="E38" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="63"/>
+      <c r="G38" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="64"/>
       <c r="I38" s="50" t="s">
         <v>13</v>
       </c>
@@ -2733,14 +2773,14 @@
       <c r="D39" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="54"/>
-      <c r="G39" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="55"/>
+      <c r="E39" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="63"/>
+      <c r="G39" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="64"/>
       <c r="I39" s="50" t="s">
         <v>13</v>
       </c>
@@ -2762,14 +2802,14 @@
       <c r="D40" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="54"/>
-      <c r="G40" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="55"/>
+      <c r="E40" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="63"/>
+      <c r="G40" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="64"/>
       <c r="I40" s="50" t="s">
         <v>13</v>
       </c>
@@ -2791,14 +2831,14 @@
       <c r="D41" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="54"/>
-      <c r="G41" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="55"/>
+      <c r="E41" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="63"/>
+      <c r="G41" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="64"/>
       <c r="I41" s="50" t="s">
         <v>13</v>
       </c>
@@ -2820,14 +2860,14 @@
       <c r="D42" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="55"/>
+      <c r="E42" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="63"/>
+      <c r="G42" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="64"/>
       <c r="I42" s="50" t="s">
         <v>13</v>
       </c>
@@ -2849,14 +2889,14 @@
       <c r="D43" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="55"/>
+      <c r="E43" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="63"/>
+      <c r="G43" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="64"/>
       <c r="I43" s="50" t="s">
         <v>13</v>
       </c>
@@ -2878,14 +2918,14 @@
       <c r="D44" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="54"/>
-      <c r="G44" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="55"/>
+      <c r="E44" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="63"/>
+      <c r="G44" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="64"/>
       <c r="I44" s="50" t="s">
         <v>13</v>
       </c>
@@ -2907,14 +2947,14 @@
       <c r="D45" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E45" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="54"/>
-      <c r="G45" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="55"/>
+      <c r="E45" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="63"/>
+      <c r="G45" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="64"/>
       <c r="I45" s="50" t="s">
         <v>13</v>
       </c>
@@ -2936,14 +2976,14 @@
       <c r="D46" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="54"/>
-      <c r="G46" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="55"/>
+      <c r="E46" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="63"/>
+      <c r="G46" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="64"/>
       <c r="I46" s="50" t="s">
         <v>13</v>
       </c>
@@ -2965,14 +3005,14 @@
       <c r="D47" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="54"/>
-      <c r="G47" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="55"/>
+      <c r="E47" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="63"/>
+      <c r="G47" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="64"/>
       <c r="I47" s="50" t="s">
         <v>13</v>
       </c>
@@ -2994,14 +3034,14 @@
       <c r="D48" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="54"/>
-      <c r="G48" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="55"/>
+      <c r="E48" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="63"/>
+      <c r="G48" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="64"/>
       <c r="I48" s="50" t="s">
         <v>13</v>
       </c>
@@ -3023,14 +3063,14 @@
       <c r="D49" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="54"/>
-      <c r="G49" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="55"/>
+      <c r="E49" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="63"/>
+      <c r="G49" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="64"/>
       <c r="I49" s="50" t="s">
         <v>13</v>
       </c>
@@ -3052,14 +3092,14 @@
       <c r="D50" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="54"/>
-      <c r="G50" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="55"/>
+      <c r="E50" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="63"/>
+      <c r="G50" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="64"/>
       <c r="I50" s="50" t="s">
         <v>13</v>
       </c>
@@ -3081,14 +3121,14 @@
       <c r="D51" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="54"/>
-      <c r="G51" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="55"/>
+      <c r="E51" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="63"/>
+      <c r="G51" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="64"/>
       <c r="I51" s="50" t="s">
         <v>13</v>
       </c>
@@ -3110,14 +3150,14 @@
       <c r="D52" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="54"/>
-      <c r="G52" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="55"/>
+      <c r="E52" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="63"/>
+      <c r="G52" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="64"/>
       <c r="I52" s="50" t="s">
         <v>13</v>
       </c>
@@ -3139,14 +3179,14 @@
       <c r="D53" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="54"/>
-      <c r="G53" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H53" s="55"/>
+      <c r="E53" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="63"/>
+      <c r="G53" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="64"/>
       <c r="I53" s="50" t="s">
         <v>13</v>
       </c>
@@ -3168,14 +3208,14 @@
       <c r="D54" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="54"/>
-      <c r="G54" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="55"/>
+      <c r="E54" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="63"/>
+      <c r="G54" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="64"/>
       <c r="I54" s="50" t="s">
         <v>13</v>
       </c>
@@ -3197,14 +3237,14 @@
       <c r="D55" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="54"/>
-      <c r="G55" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H55" s="55"/>
+      <c r="E55" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="63"/>
+      <c r="G55" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="64"/>
       <c r="I55" s="50" t="s">
         <v>13</v>
       </c>
@@ -3226,14 +3266,14 @@
       <c r="D56" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="54"/>
-      <c r="G56" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H56" s="55"/>
+      <c r="E56" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="63"/>
+      <c r="G56" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="64"/>
       <c r="I56" s="50" t="s">
         <v>13</v>
       </c>
@@ -3255,14 +3295,14 @@
       <c r="D57" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="54"/>
-      <c r="G57" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="55"/>
+      <c r="E57" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="63"/>
+      <c r="G57" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="64"/>
       <c r="I57" s="50" t="s">
         <v>13</v>
       </c>
@@ -3284,14 +3324,14 @@
       <c r="D58" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="54"/>
-      <c r="G58" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="55"/>
+      <c r="E58" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="63"/>
+      <c r="G58" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="64"/>
       <c r="I58" s="50" t="s">
         <v>13</v>
       </c>
@@ -3313,14 +3353,14 @@
       <c r="D59" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F59" s="54"/>
-      <c r="G59" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="55"/>
+      <c r="E59" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="63"/>
+      <c r="G59" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="64"/>
       <c r="I59" s="50" t="s">
         <v>13</v>
       </c>
@@ -3342,14 +3382,14 @@
       <c r="D60" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="54"/>
-      <c r="G60" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H60" s="55"/>
+      <c r="E60" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="63"/>
+      <c r="G60" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="64"/>
       <c r="I60" s="50" t="s">
         <v>13</v>
       </c>
@@ -3371,14 +3411,14 @@
       <c r="D61" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E61" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="54"/>
-      <c r="G61" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H61" s="55"/>
+      <c r="E61" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="63"/>
+      <c r="G61" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="64"/>
       <c r="I61" s="50" t="s">
         <v>13</v>
       </c>
@@ -3400,14 +3440,14 @@
       <c r="D62" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E62" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="54"/>
-      <c r="G62" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" s="55"/>
+      <c r="E62" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="63"/>
+      <c r="G62" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="64"/>
       <c r="I62" s="50" t="s">
         <v>13</v>
       </c>
@@ -3429,14 +3469,14 @@
       <c r="D63" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E63" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F63" s="54"/>
-      <c r="G63" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H63" s="55"/>
+      <c r="E63" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="63"/>
+      <c r="G63" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="64"/>
       <c r="I63" s="50" t="s">
         <v>13</v>
       </c>
@@ -3458,14 +3498,14 @@
       <c r="D64" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E64" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="54"/>
-      <c r="G64" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H64" s="55"/>
+      <c r="E64" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="63"/>
+      <c r="G64" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="64"/>
       <c r="I64" s="50" t="s">
         <v>13</v>
       </c>
@@ -3487,14 +3527,14 @@
       <c r="D65" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E65" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="54"/>
-      <c r="G65" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H65" s="55"/>
+      <c r="E65" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="63"/>
+      <c r="G65" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="64"/>
       <c r="I65" s="50" t="s">
         <v>13</v>
       </c>
@@ -3516,14 +3556,14 @@
       <c r="D66" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E66" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F66" s="54"/>
-      <c r="G66" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H66" s="55"/>
+      <c r="E66" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="63"/>
+      <c r="G66" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="64"/>
       <c r="I66" s="50" t="s">
         <v>13</v>
       </c>
@@ -3545,14 +3585,14 @@
       <c r="D67" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F67" s="54"/>
-      <c r="G67" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H67" s="55"/>
+      <c r="E67" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="63"/>
+      <c r="G67" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H67" s="64"/>
       <c r="I67" s="50" t="s">
         <v>13</v>
       </c>
@@ -3574,14 +3614,14 @@
       <c r="D68" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E68" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" s="54"/>
-      <c r="G68" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="55"/>
+      <c r="E68" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="63"/>
+      <c r="G68" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="64"/>
       <c r="I68" s="50" t="s">
         <v>13</v>
       </c>
@@ -3603,14 +3643,14 @@
       <c r="D69" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E69" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F69" s="54"/>
-      <c r="G69" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H69" s="55"/>
+      <c r="E69" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="63"/>
+      <c r="G69" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="64"/>
       <c r="I69" s="50" t="s">
         <v>13</v>
       </c>
@@ -3632,14 +3672,14 @@
       <c r="D70" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E70" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" s="54"/>
-      <c r="G70" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="55"/>
+      <c r="E70" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="63"/>
+      <c r="G70" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H70" s="64"/>
       <c r="I70" s="50" t="s">
         <v>13</v>
       </c>
@@ -3661,14 +3701,14 @@
       <c r="D71" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="54"/>
-      <c r="G71" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" s="55"/>
+      <c r="E71" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="63"/>
+      <c r="G71" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="64"/>
       <c r="I71" s="50" t="s">
         <v>13</v>
       </c>
@@ -3690,14 +3730,14 @@
       <c r="D72" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F72" s="54"/>
-      <c r="G72" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72" s="55"/>
+      <c r="E72" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="63"/>
+      <c r="G72" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="64"/>
       <c r="I72" s="50" t="s">
         <v>13</v>
       </c>
@@ -3719,14 +3759,14 @@
       <c r="D73" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E73" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F73" s="54"/>
-      <c r="G73" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="55"/>
+      <c r="E73" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="63"/>
+      <c r="G73" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="64"/>
       <c r="I73" s="50" t="s">
         <v>13</v>
       </c>
@@ -3748,14 +3788,14 @@
       <c r="D74" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E74" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F74" s="54"/>
-      <c r="G74" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" s="55"/>
+      <c r="E74" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="63"/>
+      <c r="G74" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="64"/>
       <c r="I74" s="50" t="s">
         <v>13</v>
       </c>
@@ -3777,14 +3817,14 @@
       <c r="D75" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E75" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75" s="54"/>
-      <c r="G75" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H75" s="55"/>
+      <c r="E75" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="63"/>
+      <c r="G75" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="64"/>
       <c r="I75" s="50" t="s">
         <v>13</v>
       </c>
@@ -3794,6 +3834,136 @@
     </row>
   </sheetData>
   <mergeCells count="147">
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:I8"/>
@@ -3811,136 +3981,6 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="G73:H73"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3956,26 +3996,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="9" customWidth="1"/>
-    <col min="2" max="4" width="24.83203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="38.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="32.83203125" style="10" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="40" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
+      <c r="A1" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="39"/>
       <c r="E1" s="43"/>
     </row>
@@ -3983,135 +4025,86 @@
       <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B8" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="C8" s="102"/>
+      <c r="D8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="45">
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="45">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45">
-        <f>IF(B6 &lt;&gt; "", A5+1, "")</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="45">
-        <f t="shared" ref="A7:A63" si="0">IF(B7 &lt;&gt; "", A6+1, "")</f>
-        <v>3</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="45">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>13</v>
-      </c>
+      <c r="B9" s="103" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="104"/>
       <c r="D9" s="26" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B10 &lt;&gt; "", A9+1, "")</f>
+        <v>2</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="104"/>
       <c r="D10" s="26" t="s">
         <v>13</v>
       </c>
@@ -4121,15 +4114,13 @@
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="45">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B11 &lt;&gt; "", A10+1, "")</f>
+        <v>3</v>
+      </c>
+      <c r="B11" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="104"/>
       <c r="D11" s="26" t="s">
         <v>13</v>
       </c>
@@ -4139,15 +4130,13 @@
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="45">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B12 &lt;&gt; "", A11+1, "")</f>
+        <v>4</v>
+      </c>
+      <c r="B12" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="104"/>
       <c r="D12" s="26" t="s">
         <v>13</v>
       </c>
@@ -4157,15 +4146,13 @@
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="45">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B13 &lt;&gt; "", A12+1, "")</f>
+        <v>5</v>
+      </c>
+      <c r="B13" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="104"/>
       <c r="D13" s="26" t="s">
         <v>13</v>
       </c>
@@ -4175,15 +4162,13 @@
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="45">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B14 &lt;&gt; "", A13+1, "")</f>
+        <v>6</v>
+      </c>
+      <c r="B14" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="104"/>
       <c r="D14" s="26" t="s">
         <v>13</v>
       </c>
@@ -4193,15 +4178,13 @@
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="45">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B15 &lt;&gt; "", A14+1, "")</f>
+        <v>7</v>
+      </c>
+      <c r="B15" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="104"/>
       <c r="D15" s="26" t="s">
         <v>13</v>
       </c>
@@ -4211,15 +4194,13 @@
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="45">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B16 &lt;&gt; "", A15+1, "")</f>
+        <v>8</v>
+      </c>
+      <c r="B16" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="104"/>
       <c r="D16" s="26" t="s">
         <v>13</v>
       </c>
@@ -4229,15 +4210,13 @@
     </row>
     <row r="17" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="45">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B17 &lt;&gt; "", A16+1, "")</f>
+        <v>9</v>
+      </c>
+      <c r="B17" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="104"/>
       <c r="D17" s="26" t="s">
         <v>13</v>
       </c>
@@ -4247,15 +4226,13 @@
     </row>
     <row r="18" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="45">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B18 &lt;&gt; "", A17+1, "")</f>
+        <v>10</v>
+      </c>
+      <c r="B18" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="104"/>
       <c r="D18" s="26" t="s">
         <v>13</v>
       </c>
@@ -4265,15 +4242,13 @@
     </row>
     <row r="19" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="45">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B19 &lt;&gt; "", A18+1, "")</f>
+        <v>11</v>
+      </c>
+      <c r="B19" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="104"/>
       <c r="D19" s="26" t="s">
         <v>13</v>
       </c>
@@ -4283,15 +4258,13 @@
     </row>
     <row r="20" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B20 &lt;&gt; "", A19+1, "")</f>
+        <v>12</v>
+      </c>
+      <c r="B20" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="104"/>
       <c r="D20" s="26" t="s">
         <v>13</v>
       </c>
@@ -4301,15 +4274,13 @@
     </row>
     <row r="21" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="45">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B21 &lt;&gt; "", A20+1, "")</f>
+        <v>13</v>
+      </c>
+      <c r="B21" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="104"/>
       <c r="D21" s="26" t="s">
         <v>13</v>
       </c>
@@ -4319,15 +4290,13 @@
     </row>
     <row r="22" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="45">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B22 &lt;&gt; "", A21+1, "")</f>
+        <v>14</v>
+      </c>
+      <c r="B22" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="104"/>
       <c r="D22" s="26" t="s">
         <v>13</v>
       </c>
@@ -4337,15 +4306,13 @@
     </row>
     <row r="23" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="45">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B23 &lt;&gt; "", A22+1, "")</f>
+        <v>15</v>
+      </c>
+      <c r="B23" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="104"/>
       <c r="D23" s="26" t="s">
         <v>13</v>
       </c>
@@ -4355,15 +4322,13 @@
     </row>
     <row r="24" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="45">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B24 &lt;&gt; "", A23+1, "")</f>
+        <v>16</v>
+      </c>
+      <c r="B24" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="104"/>
       <c r="D24" s="26" t="s">
         <v>13</v>
       </c>
@@ -4373,15 +4338,13 @@
     </row>
     <row r="25" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="45">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B25 &lt;&gt; "", A24+1, "")</f>
+        <v>17</v>
+      </c>
+      <c r="B25" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="104"/>
       <c r="D25" s="26" t="s">
         <v>13</v>
       </c>
@@ -4391,15 +4354,13 @@
     </row>
     <row r="26" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="45">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B26 &lt;&gt; "", A25+1, "")</f>
+        <v>18</v>
+      </c>
+      <c r="B26" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="104"/>
       <c r="D26" s="26" t="s">
         <v>13</v>
       </c>
@@ -4409,15 +4370,13 @@
     </row>
     <row r="27" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B27 &lt;&gt; "", A26+1, "")</f>
+        <v>19</v>
+      </c>
+      <c r="B27" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="104"/>
       <c r="D27" s="26" t="s">
         <v>13</v>
       </c>
@@ -4427,15 +4386,13 @@
     </row>
     <row r="28" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B28 &lt;&gt; "", A27+1, "")</f>
+        <v>20</v>
+      </c>
+      <c r="B28" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="104"/>
       <c r="D28" s="26" t="s">
         <v>13</v>
       </c>
@@ -4445,15 +4402,13 @@
     </row>
     <row r="29" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="45">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B29 &lt;&gt; "", A28+1, "")</f>
+        <v>21</v>
+      </c>
+      <c r="B29" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="104"/>
       <c r="D29" s="26" t="s">
         <v>13</v>
       </c>
@@ -4463,15 +4418,13 @@
     </row>
     <row r="30" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="45">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B30 &lt;&gt; "", A29+1, "")</f>
+        <v>22</v>
+      </c>
+      <c r="B30" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="104"/>
       <c r="D30" s="26" t="s">
         <v>13</v>
       </c>
@@ -4481,15 +4434,13 @@
     </row>
     <row r="31" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="45">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B31 &lt;&gt; "", A30+1, "")</f>
+        <v>23</v>
+      </c>
+      <c r="B31" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="104"/>
       <c r="D31" s="26" t="s">
         <v>13</v>
       </c>
@@ -4499,15 +4450,13 @@
     </row>
     <row r="32" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B32 &lt;&gt; "", A31+1, "")</f>
+        <v>24</v>
+      </c>
+      <c r="B32" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="104"/>
       <c r="D32" s="26" t="s">
         <v>13</v>
       </c>
@@ -4517,15 +4466,13 @@
     </row>
     <row r="33" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="45">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B33 &lt;&gt; "", A32+1, "")</f>
+        <v>25</v>
+      </c>
+      <c r="B33" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="104"/>
       <c r="D33" s="26" t="s">
         <v>13</v>
       </c>
@@ -4535,15 +4482,13 @@
     </row>
     <row r="34" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B34 &lt;&gt; "", A33+1, "")</f>
+        <v>26</v>
+      </c>
+      <c r="B34" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="104"/>
       <c r="D34" s="26" t="s">
         <v>13</v>
       </c>
@@ -4553,15 +4498,13 @@
     </row>
     <row r="35" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="45">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B35 &lt;&gt; "", A34+1, "")</f>
+        <v>27</v>
+      </c>
+      <c r="B35" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="104"/>
       <c r="D35" s="26" t="s">
         <v>13</v>
       </c>
@@ -4571,15 +4514,13 @@
     </row>
     <row r="36" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="45">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B36 &lt;&gt; "", A35+1, "")</f>
+        <v>28</v>
+      </c>
+      <c r="B36" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="104"/>
       <c r="D36" s="26" t="s">
         <v>13</v>
       </c>
@@ -4589,15 +4530,13 @@
     </row>
     <row r="37" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="45">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B37 &lt;&gt; "", A36+1, "")</f>
+        <v>29</v>
+      </c>
+      <c r="B37" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="104"/>
       <c r="D37" s="26" t="s">
         <v>13</v>
       </c>
@@ -4607,15 +4546,13 @@
     </row>
     <row r="38" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B38 &lt;&gt; "", A37+1, "")</f>
+        <v>30</v>
+      </c>
+      <c r="B38" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="104"/>
       <c r="D38" s="26" t="s">
         <v>13</v>
       </c>
@@ -4625,15 +4562,13 @@
     </row>
     <row r="39" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="45">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B39 &lt;&gt; "", A38+1, "")</f>
+        <v>31</v>
+      </c>
+      <c r="B39" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="104"/>
       <c r="D39" s="26" t="s">
         <v>13</v>
       </c>
@@ -4643,15 +4578,13 @@
     </row>
     <row r="40" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="45">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B40 &lt;&gt; "", A39+1, "")</f>
+        <v>32</v>
+      </c>
+      <c r="B40" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="104"/>
       <c r="D40" s="26" t="s">
         <v>13</v>
       </c>
@@ -4661,15 +4594,13 @@
     </row>
     <row r="41" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="45">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B41 &lt;&gt; "", A40+1, "")</f>
+        <v>33</v>
+      </c>
+      <c r="B41" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="104"/>
       <c r="D41" s="26" t="s">
         <v>13</v>
       </c>
@@ -4679,15 +4610,13 @@
     </row>
     <row r="42" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="45">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B42 &lt;&gt; "", A41+1, "")</f>
+        <v>34</v>
+      </c>
+      <c r="B42" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="104"/>
       <c r="D42" s="26" t="s">
         <v>13</v>
       </c>
@@ -4697,15 +4626,13 @@
     </row>
     <row r="43" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="45">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B43 &lt;&gt; "", A42+1, "")</f>
+        <v>35</v>
+      </c>
+      <c r="B43" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="104"/>
       <c r="D43" s="26" t="s">
         <v>13</v>
       </c>
@@ -4715,15 +4642,13 @@
     </row>
     <row r="44" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="45">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B44 &lt;&gt; "", A43+1, "")</f>
+        <v>36</v>
+      </c>
+      <c r="B44" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="104"/>
       <c r="D44" s="26" t="s">
         <v>13</v>
       </c>
@@ -4733,15 +4658,13 @@
     </row>
     <row r="45" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="45">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B45 &lt;&gt; "", A44+1, "")</f>
+        <v>37</v>
+      </c>
+      <c r="B45" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="104"/>
       <c r="D45" s="26" t="s">
         <v>13</v>
       </c>
@@ -4751,15 +4674,13 @@
     </row>
     <row r="46" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="45">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B46 &lt;&gt; "", A45+1, "")</f>
+        <v>38</v>
+      </c>
+      <c r="B46" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="104"/>
       <c r="D46" s="26" t="s">
         <v>13</v>
       </c>
@@ -4769,15 +4690,13 @@
     </row>
     <row r="47" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="45">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B47 &lt;&gt; "", A46+1, "")</f>
+        <v>39</v>
+      </c>
+      <c r="B47" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="104"/>
       <c r="D47" s="26" t="s">
         <v>13</v>
       </c>
@@ -4787,15 +4706,13 @@
     </row>
     <row r="48" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B48 &lt;&gt; "", A47+1, "")</f>
+        <v>40</v>
+      </c>
+      <c r="B48" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="104"/>
       <c r="D48" s="26" t="s">
         <v>13</v>
       </c>
@@ -4805,15 +4722,13 @@
     </row>
     <row r="49" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="45">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B49 &lt;&gt; "", A48+1, "")</f>
+        <v>41</v>
+      </c>
+      <c r="B49" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="104"/>
       <c r="D49" s="26" t="s">
         <v>13</v>
       </c>
@@ -4823,15 +4738,13 @@
     </row>
     <row r="50" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="45">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B50 &lt;&gt; "", A49+1, "")</f>
+        <v>42</v>
+      </c>
+      <c r="B50" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="104"/>
       <c r="D50" s="26" t="s">
         <v>13</v>
       </c>
@@ -4841,15 +4754,13 @@
     </row>
     <row r="51" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="45">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B51 &lt;&gt; "", A50+1, "")</f>
+        <v>43</v>
+      </c>
+      <c r="B51" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="104"/>
       <c r="D51" s="26" t="s">
         <v>13</v>
       </c>
@@ -4859,15 +4770,13 @@
     </row>
     <row r="52" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="45">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B52 &lt;&gt; "", A51+1, "")</f>
+        <v>44</v>
+      </c>
+      <c r="B52" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="104"/>
       <c r="D52" s="26" t="s">
         <v>13</v>
       </c>
@@ -4877,15 +4786,13 @@
     </row>
     <row r="53" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="45">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B53 &lt;&gt; "", A52+1, "")</f>
+        <v>45</v>
+      </c>
+      <c r="B53" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="104"/>
       <c r="D53" s="26" t="s">
         <v>13</v>
       </c>
@@ -4895,15 +4802,13 @@
     </row>
     <row r="54" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="45">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B54 &lt;&gt; "", A53+1, "")</f>
+        <v>46</v>
+      </c>
+      <c r="B54" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="104"/>
       <c r="D54" s="26" t="s">
         <v>13</v>
       </c>
@@ -4913,15 +4818,13 @@
     </row>
     <row r="55" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="45">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B55 &lt;&gt; "", A54+1, "")</f>
+        <v>47</v>
+      </c>
+      <c r="B55" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="104"/>
       <c r="D55" s="26" t="s">
         <v>13</v>
       </c>
@@ -4931,15 +4834,13 @@
     </row>
     <row r="56" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="45">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B56 &lt;&gt; "", A55+1, "")</f>
+        <v>48</v>
+      </c>
+      <c r="B56" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="104"/>
       <c r="D56" s="26" t="s">
         <v>13</v>
       </c>
@@ -4949,15 +4850,13 @@
     </row>
     <row r="57" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="45">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B57 &lt;&gt; "", A56+1, "")</f>
+        <v>49</v>
+      </c>
+      <c r="B57" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="104"/>
       <c r="D57" s="26" t="s">
         <v>13</v>
       </c>
@@ -4967,15 +4866,13 @@
     </row>
     <row r="58" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="45">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B58 &lt;&gt; "", A57+1, "")</f>
+        <v>50</v>
+      </c>
+      <c r="B58" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="104"/>
       <c r="D58" s="26" t="s">
         <v>13</v>
       </c>
@@ -4985,15 +4882,13 @@
     </row>
     <row r="59" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="45">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B59 &lt;&gt; "", A58+1, "")</f>
+        <v>51</v>
+      </c>
+      <c r="B59" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="104"/>
       <c r="D59" s="26" t="s">
         <v>13</v>
       </c>
@@ -5003,15 +4898,13 @@
     </row>
     <row r="60" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="45">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B60 &lt;&gt; "", A59+1, "")</f>
+        <v>52</v>
+      </c>
+      <c r="B60" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="104"/>
       <c r="D60" s="26" t="s">
         <v>13</v>
       </c>
@@ -5021,15 +4914,13 @@
     </row>
     <row r="61" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="45">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C61" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B61 &lt;&gt; "", A60+1, "")</f>
+        <v>53</v>
+      </c>
+      <c r="B61" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="104"/>
       <c r="D61" s="26" t="s">
         <v>13</v>
       </c>
@@ -5039,15 +4930,13 @@
     </row>
     <row r="62" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="45">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" s="26" t="s">
-        <v>13</v>
-      </c>
+        <f>IF(B62 &lt;&gt; "", A61+1, "")</f>
+        <v>54</v>
+      </c>
+      <c r="B62" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="104"/>
       <c r="D62" s="26" t="s">
         <v>13</v>
       </c>
@@ -5057,25 +4946,146 @@
     </row>
     <row r="63" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="45">
-        <f t="shared" si="0"/>
+        <f>IF(B63 &lt;&gt; "", A62+1, "")</f>
+        <v>55</v>
+      </c>
+      <c r="B63" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="104"/>
+      <c r="D63" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="45">
+        <f>IF(B64 &lt;&gt; "", A63+1, "")</f>
+        <v>56</v>
+      </c>
+      <c r="B64" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="104"/>
+      <c r="D64" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="45">
+        <f>IF(B65 &lt;&gt; "", A64+1, "")</f>
+        <v>57</v>
+      </c>
+      <c r="B65" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="104"/>
+      <c r="D65" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="45">
+        <f>IF(B66 &lt;&gt; "", A65+1, "")</f>
+        <v>58</v>
+      </c>
+      <c r="B66" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="104"/>
+      <c r="D66" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="45">
+        <f>IF(B67 &lt;&gt; "", A66+1, "")</f>
         <v>59</v>
       </c>
-      <c r="B63" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E63" s="26" t="s">
+      <c r="B67" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="104"/>
+      <c r="D67" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="26" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="60">
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -5105,11 +5115,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="42" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
       <c r="D1" s="40"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
@@ -5146,10 +5156,10 @@
       <c r="D3" s="16"/>
       <c r="E3" s="1"/>
       <c r="F3" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H3" s="17"/>
       <c r="I3" s="1"/>
@@ -5159,46 +5169,46 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="86" t="s">
+      <c r="H4" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84" t="s">
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="97"/>
+      <c r="A5" s="93"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="99"/>
       <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
@@ -5211,7 +5221,7 @@
       <c r="K5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="85"/>
+      <c r="L5" s="87"/>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="95" x14ac:dyDescent="0.3">
@@ -5231,10 +5241,10 @@
         <v>19</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>33</v>
@@ -7638,8 +7648,8 @@
   </sheetPr>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -7655,17 +7665,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="40" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
-      <c r="F1" s="98" t="s">
+      <c r="F1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="98"/>
+      <c r="G1" s="100"/>
       <c r="H1" s="39"/>
       <c r="I1" s="43"/>
       <c r="J1" s="43"/>
@@ -7738,37 +7748,37 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="F5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="K5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="45">
         <f>IF(B6 &lt;&gt; "", A5+1, "")</f>
         <v>2</v>
@@ -7804,7 +7814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="45">
         <f t="shared" ref="A7:A63" si="0">IF(B7 &lt;&gt; "", A6+1, "")</f>
         <v>3</v>
@@ -7840,7 +7850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7876,7 +7886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7912,7 +7922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="45">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7948,7 +7958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="45">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7984,7 +7994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="45">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8020,7 +8030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="45">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8056,7 +8066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="45">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8092,7 +8102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="45">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8128,7 +8138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="45">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -8164,7 +8174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="45">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -8200,7 +8210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="45">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8236,7 +8246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="45">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8272,7 +8282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="45">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8308,7 +8318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="45">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8344,7 +8354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="45">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -8380,7 +8390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" s="45">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -8416,7 +8426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="45">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -8452,7 +8462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="45">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -8488,7 +8498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="45">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -8524,7 +8534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="45">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -8560,7 +8570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="45">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -8596,7 +8606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="45">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -8632,7 +8642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="45">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -8668,7 +8678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="45">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -8704,7 +8714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="45">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -8740,7 +8750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="45">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -8776,7 +8786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="45">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8812,7 +8822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="45">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -8848,7 +8858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" s="45">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -8884,7 +8894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" s="45">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -8920,7 +8930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="45">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -8956,7 +8966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A39" s="45">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -8992,7 +9002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" s="45">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -9028,7 +9038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" s="45">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -9064,7 +9074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A42" s="45">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -9100,7 +9110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A43" s="45">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -9136,7 +9146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A44" s="45">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -9172,7 +9182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A45" s="45">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -9208,7 +9218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A46" s="45">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9244,7 +9254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A47" s="45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9280,7 +9290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9316,7 +9326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A49" s="45">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9352,7 +9362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A50" s="45">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9388,7 +9398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A51" s="45">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9424,7 +9434,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A52" s="45">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9460,7 +9470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A53" s="45">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9496,7 +9506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A54" s="45">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9532,7 +9542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A55" s="45">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -9568,7 +9578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A56" s="45">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -9604,7 +9614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A57" s="45">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -9640,7 +9650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" s="45">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -9676,7 +9686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A59" s="45">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -9712,7 +9722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A60" s="45">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -9748,7 +9758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A61" s="45">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -9784,7 +9794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A62" s="45">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -9820,7 +9830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A63" s="45">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -9871,34 +9881,34 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="255.6640625" style="100" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="100"/>
+    <col min="1" max="1" width="255.6640625" style="54" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="220" x14ac:dyDescent="0.2">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="53" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="53" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="400" x14ac:dyDescent="0.2">
-      <c r="A3" s="99" t="s">
-        <v>43</v>
+      <c r="A3" s="53" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="260" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
-        <v>74</v>
+      <c r="A4" s="53" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>